<commit_message>
APS-220 added convenience function to search for enums
</commit_message>
<xml_diff>
--- a/persistence-utils-demo-tool/src/com/axonivy/utils/persistence/demo/tool/test/testdata/testdata.xlsx
+++ b/persistence-utils-demo-tool/src/com/axonivy/utils/persistence/demo/tool/test/testdata/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\AxonIvy\demos\bp\ws\bp\bp_test\src\com\axonivy\demo\bp\test\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\AxonIvy\marketplace\persistence\ws\persistence-utils-modules\persistence-utils-demo-tool\src\com\axonivy\utils\persistence\demo\tool\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F223BCC2-E115-4930-AD81-0299E01B19CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A22C271-63CE-4E22-ADD8-DAB38D31A848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7725" yWindow="3780" windowWidth="30870" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="24945" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4109" uniqueCount="1702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4109" uniqueCount="1703">
   <si>
     <t>ID</t>
   </si>
@@ -5127,6 +5127,9 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>PARTNER_PASSED_AWAY</t>
   </si>
 </sst>
 </file>
@@ -5242,9 +5245,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5282,7 +5285,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5388,7 +5391,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5530,7 +5533,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5711,8 +5714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D347" workbookViewId="0">
-      <selection activeCell="L374" sqref="L374"/>
+    <sheetView tabSelected="1" topLeftCell="E272" workbookViewId="0">
+      <selection activeCell="M274" sqref="M274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17785,7 +17788,7 @@
         <v>1007</v>
       </c>
       <c r="M274" t="s">
-        <v>1364</v>
+        <v>1702</v>
       </c>
       <c r="N274" t="s">
         <v>1700</v>
@@ -19369,7 +19372,7 @@
         <v>1132</v>
       </c>
       <c r="M310" t="s">
-        <v>1364</v>
+        <v>1702</v>
       </c>
       <c r="N310" t="s">
         <v>1700</v>

</xml_diff>